<commit_message>
timer, ociosidade, font e etc
</commit_message>
<xml_diff>
--- a/registration_data.xlsx
+++ b/registration_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H98"/>
+  <dimension ref="A1:H166"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4541,6 +4541,2862 @@
         </is>
       </c>
     </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>Nome e Sobrenome:</t>
+        </is>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>Email:</t>
+        </is>
+      </c>
+      <c r="C99" t="inlineStr">
+        <is>
+          <t>Celular:</t>
+        </is>
+      </c>
+      <c r="D99" t="inlineStr">
+        <is>
+          <t>Cidade:</t>
+        </is>
+      </c>
+      <c r="E99" t="inlineStr">
+        <is>
+          <t>UF:</t>
+        </is>
+      </c>
+      <c r="F99" t="inlineStr">
+        <is>
+          <t>Empresa:</t>
+        </is>
+      </c>
+      <c r="G99" t="inlineStr">
+        <is>
+          <t>Segmento:</t>
+        </is>
+      </c>
+      <c r="H99" t="inlineStr">
+        <is>
+          <t>CNPJ:</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>Name and Last Name:</t>
+        </is>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>Email:</t>
+        </is>
+      </c>
+      <c r="C100" t="inlineStr">
+        <is>
+          <t>Phone:</t>
+        </is>
+      </c>
+      <c r="D100" t="inlineStr">
+        <is>
+          <t>City:</t>
+        </is>
+      </c>
+      <c r="E100" t="inlineStr">
+        <is>
+          <t>State:</t>
+        </is>
+      </c>
+      <c r="F100" t="inlineStr">
+        <is>
+          <t>Company:</t>
+        </is>
+      </c>
+      <c r="G100" t="inlineStr">
+        <is>
+          <t>Segment:</t>
+        </is>
+      </c>
+      <c r="H100" t="inlineStr">
+        <is>
+          <t>CNPJ:</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>Nome e Sobrenome:</t>
+        </is>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>Email:</t>
+        </is>
+      </c>
+      <c r="C101" t="inlineStr">
+        <is>
+          <t>Celular:</t>
+        </is>
+      </c>
+      <c r="D101" t="inlineStr">
+        <is>
+          <t>Cidade:</t>
+        </is>
+      </c>
+      <c r="E101" t="inlineStr">
+        <is>
+          <t>UF:</t>
+        </is>
+      </c>
+      <c r="F101" t="inlineStr">
+        <is>
+          <t>Empresa:</t>
+        </is>
+      </c>
+      <c r="G101" t="inlineStr">
+        <is>
+          <t>Segmento:</t>
+        </is>
+      </c>
+      <c r="H101" t="inlineStr">
+        <is>
+          <t>CNPJ:</t>
+        </is>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>Name and Last Name:</t>
+        </is>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>Email:</t>
+        </is>
+      </c>
+      <c r="C102" t="inlineStr">
+        <is>
+          <t>Phone:</t>
+        </is>
+      </c>
+      <c r="D102" t="inlineStr">
+        <is>
+          <t>City:</t>
+        </is>
+      </c>
+      <c r="E102" t="inlineStr">
+        <is>
+          <t>State:</t>
+        </is>
+      </c>
+      <c r="F102" t="inlineStr">
+        <is>
+          <t>Company:</t>
+        </is>
+      </c>
+      <c r="G102" t="inlineStr">
+        <is>
+          <t>Segment:</t>
+        </is>
+      </c>
+      <c r="H102" t="inlineStr">
+        <is>
+          <t>CNPJ:</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>Name and Last Name:</t>
+        </is>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>Email:</t>
+        </is>
+      </c>
+      <c r="C103" t="inlineStr">
+        <is>
+          <t>Phone:</t>
+        </is>
+      </c>
+      <c r="D103" t="inlineStr">
+        <is>
+          <t>City:</t>
+        </is>
+      </c>
+      <c r="E103" t="inlineStr">
+        <is>
+          <t>State:</t>
+        </is>
+      </c>
+      <c r="F103" t="inlineStr">
+        <is>
+          <t>Company:</t>
+        </is>
+      </c>
+      <c r="G103" t="inlineStr">
+        <is>
+          <t>Segment:</t>
+        </is>
+      </c>
+      <c r="H103" t="inlineStr">
+        <is>
+          <t>CNPJ:</t>
+        </is>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>Nome e Sobrenome:</t>
+        </is>
+      </c>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t>Email:</t>
+        </is>
+      </c>
+      <c r="C104" t="inlineStr">
+        <is>
+          <t>Celular:</t>
+        </is>
+      </c>
+      <c r="D104" t="inlineStr">
+        <is>
+          <t>Cidade:</t>
+        </is>
+      </c>
+      <c r="E104" t="inlineStr">
+        <is>
+          <t>UF:</t>
+        </is>
+      </c>
+      <c r="F104" t="inlineStr">
+        <is>
+          <t>Empresa:</t>
+        </is>
+      </c>
+      <c r="G104" t="inlineStr">
+        <is>
+          <t>Segmento:</t>
+        </is>
+      </c>
+      <c r="H104" t="inlineStr">
+        <is>
+          <t>CNPJ:</t>
+        </is>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>Name and Last Name:</t>
+        </is>
+      </c>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t>Email:</t>
+        </is>
+      </c>
+      <c r="C105" t="inlineStr">
+        <is>
+          <t>Phone:</t>
+        </is>
+      </c>
+      <c r="D105" t="inlineStr">
+        <is>
+          <t>City:</t>
+        </is>
+      </c>
+      <c r="E105" t="inlineStr">
+        <is>
+          <t>State:</t>
+        </is>
+      </c>
+      <c r="F105" t="inlineStr">
+        <is>
+          <t>Company:</t>
+        </is>
+      </c>
+      <c r="G105" t="inlineStr">
+        <is>
+          <t>Segment:</t>
+        </is>
+      </c>
+      <c r="H105" t="inlineStr">
+        <is>
+          <t>CNPJ:</t>
+        </is>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr">
+        <is>
+          <t>Nome e Sobrenome:</t>
+        </is>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>Email:</t>
+        </is>
+      </c>
+      <c r="C106" t="inlineStr">
+        <is>
+          <t>Celular:</t>
+        </is>
+      </c>
+      <c r="D106" t="inlineStr">
+        <is>
+          <t>Cidade:</t>
+        </is>
+      </c>
+      <c r="E106" t="inlineStr">
+        <is>
+          <t>UF:</t>
+        </is>
+      </c>
+      <c r="F106" t="inlineStr">
+        <is>
+          <t>Empresa:</t>
+        </is>
+      </c>
+      <c r="G106" t="inlineStr">
+        <is>
+          <t>Segmento:</t>
+        </is>
+      </c>
+      <c r="H106" t="inlineStr">
+        <is>
+          <t>CNPJ:</t>
+        </is>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="inlineStr">
+        <is>
+          <t>Name and Last Name:</t>
+        </is>
+      </c>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>Email:</t>
+        </is>
+      </c>
+      <c r="C107" t="inlineStr">
+        <is>
+          <t>Phone:</t>
+        </is>
+      </c>
+      <c r="D107" t="inlineStr">
+        <is>
+          <t>City:</t>
+        </is>
+      </c>
+      <c r="E107" t="inlineStr">
+        <is>
+          <t>State:</t>
+        </is>
+      </c>
+      <c r="F107" t="inlineStr">
+        <is>
+          <t>Company:</t>
+        </is>
+      </c>
+      <c r="G107" t="inlineStr">
+        <is>
+          <t>Segment:</t>
+        </is>
+      </c>
+      <c r="H107" t="inlineStr">
+        <is>
+          <t>CNPJ:</t>
+        </is>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="inlineStr">
+        <is>
+          <t>Nome e Sobrenome:</t>
+        </is>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>Email:</t>
+        </is>
+      </c>
+      <c r="C108" t="inlineStr">
+        <is>
+          <t>Celular:</t>
+        </is>
+      </c>
+      <c r="D108" t="inlineStr">
+        <is>
+          <t>Cidade:</t>
+        </is>
+      </c>
+      <c r="E108" t="inlineStr">
+        <is>
+          <t>UF:</t>
+        </is>
+      </c>
+      <c r="F108" t="inlineStr">
+        <is>
+          <t>Empresa:</t>
+        </is>
+      </c>
+      <c r="G108" t="inlineStr">
+        <is>
+          <t>Segmento:</t>
+        </is>
+      </c>
+      <c r="H108" t="inlineStr">
+        <is>
+          <t>CNPJ:</t>
+        </is>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="inlineStr">
+        <is>
+          <t>Name and Last Name:</t>
+        </is>
+      </c>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>Email:</t>
+        </is>
+      </c>
+      <c r="C109" t="inlineStr">
+        <is>
+          <t>Phone:</t>
+        </is>
+      </c>
+      <c r="D109" t="inlineStr">
+        <is>
+          <t>City:</t>
+        </is>
+      </c>
+      <c r="E109" t="inlineStr">
+        <is>
+          <t>State:</t>
+        </is>
+      </c>
+      <c r="F109" t="inlineStr">
+        <is>
+          <t>Company:</t>
+        </is>
+      </c>
+      <c r="G109" t="inlineStr">
+        <is>
+          <t>Segment:</t>
+        </is>
+      </c>
+      <c r="H109" t="inlineStr">
+        <is>
+          <t>CNPJ:</t>
+        </is>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="inlineStr">
+        <is>
+          <t>Name and Last Name:</t>
+        </is>
+      </c>
+      <c r="B110" t="inlineStr">
+        <is>
+          <t>Email:</t>
+        </is>
+      </c>
+      <c r="C110" t="inlineStr">
+        <is>
+          <t>Phone:</t>
+        </is>
+      </c>
+      <c r="D110" t="inlineStr">
+        <is>
+          <t>City:</t>
+        </is>
+      </c>
+      <c r="E110" t="inlineStr">
+        <is>
+          <t>State:</t>
+        </is>
+      </c>
+      <c r="F110" t="inlineStr">
+        <is>
+          <t>Company:</t>
+        </is>
+      </c>
+      <c r="G110" t="inlineStr">
+        <is>
+          <t>Segment:</t>
+        </is>
+      </c>
+      <c r="H110" t="inlineStr">
+        <is>
+          <t>CNPJ:</t>
+        </is>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="inlineStr">
+        <is>
+          <t>Name and Last Name:</t>
+        </is>
+      </c>
+      <c r="B111" t="inlineStr">
+        <is>
+          <t>Email:</t>
+        </is>
+      </c>
+      <c r="C111" t="inlineStr">
+        <is>
+          <t>Phone:</t>
+        </is>
+      </c>
+      <c r="D111" t="inlineStr">
+        <is>
+          <t>City:</t>
+        </is>
+      </c>
+      <c r="E111" t="inlineStr">
+        <is>
+          <t>State:</t>
+        </is>
+      </c>
+      <c r="F111" t="inlineStr">
+        <is>
+          <t>Company:</t>
+        </is>
+      </c>
+      <c r="G111" t="inlineStr">
+        <is>
+          <t>Segment:</t>
+        </is>
+      </c>
+      <c r="H111" t="inlineStr">
+        <is>
+          <t>CNPJ:</t>
+        </is>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="inlineStr">
+        <is>
+          <t>Nome e Sobrenome:</t>
+        </is>
+      </c>
+      <c r="B112" t="inlineStr">
+        <is>
+          <t>Email:</t>
+        </is>
+      </c>
+      <c r="C112" t="inlineStr">
+        <is>
+          <t>Celular:</t>
+        </is>
+      </c>
+      <c r="D112" t="inlineStr">
+        <is>
+          <t>Cidade:</t>
+        </is>
+      </c>
+      <c r="E112" t="inlineStr">
+        <is>
+          <t>UF:</t>
+        </is>
+      </c>
+      <c r="F112" t="inlineStr">
+        <is>
+          <t>Empresa:</t>
+        </is>
+      </c>
+      <c r="G112" t="inlineStr">
+        <is>
+          <t>Segmento:</t>
+        </is>
+      </c>
+      <c r="H112" t="inlineStr">
+        <is>
+          <t>CNPJ:</t>
+        </is>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="inlineStr">
+        <is>
+          <t>Nome e Sobrenome:</t>
+        </is>
+      </c>
+      <c r="B113" t="inlineStr">
+        <is>
+          <t>Email:</t>
+        </is>
+      </c>
+      <c r="C113" t="inlineStr">
+        <is>
+          <t>Celular:</t>
+        </is>
+      </c>
+      <c r="D113" t="inlineStr">
+        <is>
+          <t>Cidade:</t>
+        </is>
+      </c>
+      <c r="E113" t="inlineStr">
+        <is>
+          <t>UF:</t>
+        </is>
+      </c>
+      <c r="F113" t="inlineStr">
+        <is>
+          <t>Empresa:</t>
+        </is>
+      </c>
+      <c r="G113" t="inlineStr">
+        <is>
+          <t>Segmento:</t>
+        </is>
+      </c>
+      <c r="H113" t="inlineStr">
+        <is>
+          <t>CNPJ:</t>
+        </is>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="inlineStr">
+        <is>
+          <t>Nome e Sobrenome:</t>
+        </is>
+      </c>
+      <c r="B114" t="inlineStr">
+        <is>
+          <t>Email:</t>
+        </is>
+      </c>
+      <c r="C114" t="inlineStr">
+        <is>
+          <t>Celular:</t>
+        </is>
+      </c>
+      <c r="D114" t="inlineStr">
+        <is>
+          <t>Cidade:</t>
+        </is>
+      </c>
+      <c r="E114" t="inlineStr">
+        <is>
+          <t>UF:</t>
+        </is>
+      </c>
+      <c r="F114" t="inlineStr">
+        <is>
+          <t>Empresa:</t>
+        </is>
+      </c>
+      <c r="G114" t="inlineStr">
+        <is>
+          <t>Segmento:</t>
+        </is>
+      </c>
+      <c r="H114" t="inlineStr">
+        <is>
+          <t>CNPJ:</t>
+        </is>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="inlineStr">
+        <is>
+          <t>Nome e Sobrenome:</t>
+        </is>
+      </c>
+      <c r="B115" t="inlineStr">
+        <is>
+          <t>Email:</t>
+        </is>
+      </c>
+      <c r="C115" t="inlineStr">
+        <is>
+          <t>Celular:</t>
+        </is>
+      </c>
+      <c r="D115" t="inlineStr">
+        <is>
+          <t>Cidade:</t>
+        </is>
+      </c>
+      <c r="E115" t="inlineStr">
+        <is>
+          <t>UF:</t>
+        </is>
+      </c>
+      <c r="F115" t="inlineStr">
+        <is>
+          <t>Empresa:</t>
+        </is>
+      </c>
+      <c r="G115" t="inlineStr">
+        <is>
+          <t>Segmento:</t>
+        </is>
+      </c>
+      <c r="H115" t="inlineStr">
+        <is>
+          <t>CNPJ:</t>
+        </is>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="inlineStr">
+        <is>
+          <t>Nome e Sobrenome:</t>
+        </is>
+      </c>
+      <c r="B116" t="inlineStr">
+        <is>
+          <t>Email:</t>
+        </is>
+      </c>
+      <c r="C116" t="inlineStr">
+        <is>
+          <t>Celular:</t>
+        </is>
+      </c>
+      <c r="D116" t="inlineStr">
+        <is>
+          <t>Cidade:</t>
+        </is>
+      </c>
+      <c r="E116" t="inlineStr">
+        <is>
+          <t>UF:</t>
+        </is>
+      </c>
+      <c r="F116" t="inlineStr">
+        <is>
+          <t>Empresa:</t>
+        </is>
+      </c>
+      <c r="G116" t="inlineStr">
+        <is>
+          <t>Segmento:</t>
+        </is>
+      </c>
+      <c r="H116" t="inlineStr">
+        <is>
+          <t>CNPJ:</t>
+        </is>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="inlineStr">
+        <is>
+          <t>Nome e Sobrenome:</t>
+        </is>
+      </c>
+      <c r="B117" t="inlineStr">
+        <is>
+          <t>Email:</t>
+        </is>
+      </c>
+      <c r="C117" t="inlineStr">
+        <is>
+          <t>Celular:</t>
+        </is>
+      </c>
+      <c r="D117" t="inlineStr">
+        <is>
+          <t>Cidade:</t>
+        </is>
+      </c>
+      <c r="E117" t="inlineStr">
+        <is>
+          <t>UF:</t>
+        </is>
+      </c>
+      <c r="F117" t="inlineStr">
+        <is>
+          <t>Empresa:</t>
+        </is>
+      </c>
+      <c r="G117" t="inlineStr">
+        <is>
+          <t>Segmento:</t>
+        </is>
+      </c>
+      <c r="H117" t="inlineStr">
+        <is>
+          <t>CNPJ:</t>
+        </is>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="inlineStr">
+        <is>
+          <t>Name and Last Name:</t>
+        </is>
+      </c>
+      <c r="B118" t="inlineStr">
+        <is>
+          <t>Email:</t>
+        </is>
+      </c>
+      <c r="C118" t="inlineStr">
+        <is>
+          <t>Phone:</t>
+        </is>
+      </c>
+      <c r="D118" t="inlineStr">
+        <is>
+          <t>City:</t>
+        </is>
+      </c>
+      <c r="E118" t="inlineStr">
+        <is>
+          <t>State:</t>
+        </is>
+      </c>
+      <c r="F118" t="inlineStr">
+        <is>
+          <t>Company:</t>
+        </is>
+      </c>
+      <c r="G118" t="inlineStr">
+        <is>
+          <t>Segment:</t>
+        </is>
+      </c>
+      <c r="H118" t="inlineStr">
+        <is>
+          <t>CNPJ:</t>
+        </is>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="inlineStr">
+        <is>
+          <t>Nome e Sobrenome:</t>
+        </is>
+      </c>
+      <c r="B119" t="inlineStr">
+        <is>
+          <t>Email:</t>
+        </is>
+      </c>
+      <c r="C119" t="inlineStr">
+        <is>
+          <t>Celular:</t>
+        </is>
+      </c>
+      <c r="D119" t="inlineStr">
+        <is>
+          <t>Cidade:</t>
+        </is>
+      </c>
+      <c r="E119" t="inlineStr">
+        <is>
+          <t>UF:</t>
+        </is>
+      </c>
+      <c r="F119" t="inlineStr">
+        <is>
+          <t>Empresa:</t>
+        </is>
+      </c>
+      <c r="G119" t="inlineStr">
+        <is>
+          <t>Segmento:</t>
+        </is>
+      </c>
+      <c r="H119" t="inlineStr">
+        <is>
+          <t>CNPJ:</t>
+        </is>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="inlineStr">
+        <is>
+          <t>Name and Last Name:</t>
+        </is>
+      </c>
+      <c r="B120" t="inlineStr">
+        <is>
+          <t>Email:</t>
+        </is>
+      </c>
+      <c r="C120" t="inlineStr">
+        <is>
+          <t>Phone:</t>
+        </is>
+      </c>
+      <c r="D120" t="inlineStr">
+        <is>
+          <t>City:</t>
+        </is>
+      </c>
+      <c r="E120" t="inlineStr">
+        <is>
+          <t>State:</t>
+        </is>
+      </c>
+      <c r="F120" t="inlineStr">
+        <is>
+          <t>Company:</t>
+        </is>
+      </c>
+      <c r="G120" t="inlineStr">
+        <is>
+          <t>Segment:</t>
+        </is>
+      </c>
+      <c r="H120" t="inlineStr">
+        <is>
+          <t>CNPJ:</t>
+        </is>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="inlineStr">
+        <is>
+          <t>Name and Last Name:</t>
+        </is>
+      </c>
+      <c r="B121" t="inlineStr">
+        <is>
+          <t>Email:</t>
+        </is>
+      </c>
+      <c r="C121" t="inlineStr">
+        <is>
+          <t>Phone:</t>
+        </is>
+      </c>
+      <c r="D121" t="inlineStr">
+        <is>
+          <t>City:</t>
+        </is>
+      </c>
+      <c r="E121" t="inlineStr">
+        <is>
+          <t>State:</t>
+        </is>
+      </c>
+      <c r="F121" t="inlineStr">
+        <is>
+          <t>Company:</t>
+        </is>
+      </c>
+      <c r="G121" t="inlineStr">
+        <is>
+          <t>Segment:</t>
+        </is>
+      </c>
+      <c r="H121" t="inlineStr">
+        <is>
+          <t>CNPJ:</t>
+        </is>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="inlineStr">
+        <is>
+          <t>Name and Last Name:</t>
+        </is>
+      </c>
+      <c r="B122" t="inlineStr">
+        <is>
+          <t>Email:</t>
+        </is>
+      </c>
+      <c r="C122" t="inlineStr">
+        <is>
+          <t>Phone:</t>
+        </is>
+      </c>
+      <c r="D122" t="inlineStr">
+        <is>
+          <t>City:</t>
+        </is>
+      </c>
+      <c r="E122" t="inlineStr">
+        <is>
+          <t>State:</t>
+        </is>
+      </c>
+      <c r="F122" t="inlineStr">
+        <is>
+          <t>Company:</t>
+        </is>
+      </c>
+      <c r="G122" t="inlineStr">
+        <is>
+          <t>Segment:</t>
+        </is>
+      </c>
+      <c r="H122" t="inlineStr">
+        <is>
+          <t>CNPJ:</t>
+        </is>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="inlineStr">
+        <is>
+          <t>Nome e Sobrenome:</t>
+        </is>
+      </c>
+      <c r="B123" t="inlineStr">
+        <is>
+          <t>Email:</t>
+        </is>
+      </c>
+      <c r="C123" t="inlineStr">
+        <is>
+          <t>Celular:</t>
+        </is>
+      </c>
+      <c r="D123" t="inlineStr">
+        <is>
+          <t>Cidade:</t>
+        </is>
+      </c>
+      <c r="E123" t="inlineStr">
+        <is>
+          <t>UF:</t>
+        </is>
+      </c>
+      <c r="F123" t="inlineStr">
+        <is>
+          <t>Empresa:</t>
+        </is>
+      </c>
+      <c r="G123" t="inlineStr">
+        <is>
+          <t>Segmento:</t>
+        </is>
+      </c>
+      <c r="H123" t="inlineStr">
+        <is>
+          <t>CNPJ:</t>
+        </is>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="inlineStr">
+        <is>
+          <t>Nome e Sobrenome:</t>
+        </is>
+      </c>
+      <c r="B124" t="inlineStr">
+        <is>
+          <t>Email:</t>
+        </is>
+      </c>
+      <c r="C124" t="inlineStr">
+        <is>
+          <t>Celular:</t>
+        </is>
+      </c>
+      <c r="D124" t="inlineStr">
+        <is>
+          <t>Cidade:</t>
+        </is>
+      </c>
+      <c r="E124" t="inlineStr">
+        <is>
+          <t>UF:</t>
+        </is>
+      </c>
+      <c r="F124" t="inlineStr">
+        <is>
+          <t>Empresa:</t>
+        </is>
+      </c>
+      <c r="G124" t="inlineStr">
+        <is>
+          <t>Segmento:</t>
+        </is>
+      </c>
+      <c r="H124" t="inlineStr">
+        <is>
+          <t>CNPJ:</t>
+        </is>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="inlineStr">
+        <is>
+          <t>Nome e Sobrenome:</t>
+        </is>
+      </c>
+      <c r="B125" t="inlineStr">
+        <is>
+          <t>Email:</t>
+        </is>
+      </c>
+      <c r="C125" t="inlineStr">
+        <is>
+          <t>Celular:</t>
+        </is>
+      </c>
+      <c r="D125" t="inlineStr">
+        <is>
+          <t>Cidade:</t>
+        </is>
+      </c>
+      <c r="E125" t="inlineStr">
+        <is>
+          <t>UF:</t>
+        </is>
+      </c>
+      <c r="F125" t="inlineStr">
+        <is>
+          <t>Empresa:</t>
+        </is>
+      </c>
+      <c r="G125" t="inlineStr">
+        <is>
+          <t>Segmento:</t>
+        </is>
+      </c>
+      <c r="H125" t="inlineStr">
+        <is>
+          <t>CNPJ:</t>
+        </is>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="inlineStr">
+        <is>
+          <t>Name and Last Name:</t>
+        </is>
+      </c>
+      <c r="B126" t="inlineStr">
+        <is>
+          <t>Email:</t>
+        </is>
+      </c>
+      <c r="C126" t="inlineStr">
+        <is>
+          <t>Phone:</t>
+        </is>
+      </c>
+      <c r="D126" t="inlineStr">
+        <is>
+          <t>City:</t>
+        </is>
+      </c>
+      <c r="E126" t="inlineStr">
+        <is>
+          <t>State:</t>
+        </is>
+      </c>
+      <c r="F126" t="inlineStr">
+        <is>
+          <t>Company:</t>
+        </is>
+      </c>
+      <c r="G126" t="inlineStr">
+        <is>
+          <t>Segment:</t>
+        </is>
+      </c>
+      <c r="H126" t="inlineStr">
+        <is>
+          <t>CNPJ:</t>
+        </is>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="inlineStr">
+        <is>
+          <t>Name and Last Name:</t>
+        </is>
+      </c>
+      <c r="B127" t="inlineStr">
+        <is>
+          <t>Email:</t>
+        </is>
+      </c>
+      <c r="C127" t="inlineStr">
+        <is>
+          <t>Phone:</t>
+        </is>
+      </c>
+      <c r="D127" t="inlineStr">
+        <is>
+          <t>City:</t>
+        </is>
+      </c>
+      <c r="E127" t="inlineStr">
+        <is>
+          <t>State:</t>
+        </is>
+      </c>
+      <c r="F127" t="inlineStr">
+        <is>
+          <t>Company:</t>
+        </is>
+      </c>
+      <c r="G127" t="inlineStr">
+        <is>
+          <t>Segment:</t>
+        </is>
+      </c>
+      <c r="H127" t="inlineStr">
+        <is>
+          <t>CNPJ:</t>
+        </is>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="inlineStr">
+        <is>
+          <t>Nome e Sobrenome:</t>
+        </is>
+      </c>
+      <c r="B128" t="inlineStr">
+        <is>
+          <t>Email:</t>
+        </is>
+      </c>
+      <c r="C128" t="inlineStr">
+        <is>
+          <t>Celular:</t>
+        </is>
+      </c>
+      <c r="D128" t="inlineStr">
+        <is>
+          <t>Cidade:</t>
+        </is>
+      </c>
+      <c r="E128" t="inlineStr">
+        <is>
+          <t>UF:</t>
+        </is>
+      </c>
+      <c r="F128" t="inlineStr">
+        <is>
+          <t>Empresa:</t>
+        </is>
+      </c>
+      <c r="G128" t="inlineStr">
+        <is>
+          <t>Segmento:</t>
+        </is>
+      </c>
+      <c r="H128" t="inlineStr">
+        <is>
+          <t>CNPJ:</t>
+        </is>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="inlineStr">
+        <is>
+          <t>Name and Last Name:</t>
+        </is>
+      </c>
+      <c r="B129" t="inlineStr">
+        <is>
+          <t>Email:</t>
+        </is>
+      </c>
+      <c r="C129" t="inlineStr">
+        <is>
+          <t>Phone:</t>
+        </is>
+      </c>
+      <c r="D129" t="inlineStr">
+        <is>
+          <t>City:</t>
+        </is>
+      </c>
+      <c r="E129" t="inlineStr">
+        <is>
+          <t>State:</t>
+        </is>
+      </c>
+      <c r="F129" t="inlineStr">
+        <is>
+          <t>Company:</t>
+        </is>
+      </c>
+      <c r="G129" t="inlineStr">
+        <is>
+          <t>Segment:</t>
+        </is>
+      </c>
+      <c r="H129" t="inlineStr">
+        <is>
+          <t>CNPJ:</t>
+        </is>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="inlineStr">
+        <is>
+          <t>Nome e Sobrenome:</t>
+        </is>
+      </c>
+      <c r="B130" t="inlineStr">
+        <is>
+          <t>Email:</t>
+        </is>
+      </c>
+      <c r="C130" t="inlineStr">
+        <is>
+          <t>Celular:</t>
+        </is>
+      </c>
+      <c r="D130" t="inlineStr">
+        <is>
+          <t>Cidade:</t>
+        </is>
+      </c>
+      <c r="E130" t="inlineStr">
+        <is>
+          <t>UF:</t>
+        </is>
+      </c>
+      <c r="F130" t="inlineStr">
+        <is>
+          <t>Empresa:</t>
+        </is>
+      </c>
+      <c r="G130" t="inlineStr">
+        <is>
+          <t>Segmento:</t>
+        </is>
+      </c>
+      <c r="H130" t="inlineStr">
+        <is>
+          <t>CNPJ:</t>
+        </is>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="inlineStr">
+        <is>
+          <t>Nome e Sobrenome:</t>
+        </is>
+      </c>
+      <c r="B131" t="inlineStr">
+        <is>
+          <t>Email:</t>
+        </is>
+      </c>
+      <c r="C131" t="inlineStr">
+        <is>
+          <t>Celular:</t>
+        </is>
+      </c>
+      <c r="D131" t="inlineStr">
+        <is>
+          <t>Cidade:</t>
+        </is>
+      </c>
+      <c r="E131" t="inlineStr">
+        <is>
+          <t>UF:</t>
+        </is>
+      </c>
+      <c r="F131" t="inlineStr">
+        <is>
+          <t>Empresa:</t>
+        </is>
+      </c>
+      <c r="G131" t="inlineStr">
+        <is>
+          <t>Segmento:</t>
+        </is>
+      </c>
+      <c r="H131" t="inlineStr">
+        <is>
+          <t>CNPJ:</t>
+        </is>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="inlineStr">
+        <is>
+          <t>Nome e Sobrenome:</t>
+        </is>
+      </c>
+      <c r="B132" t="inlineStr">
+        <is>
+          <t>Email:</t>
+        </is>
+      </c>
+      <c r="C132" t="inlineStr">
+        <is>
+          <t>Celular:</t>
+        </is>
+      </c>
+      <c r="D132" t="inlineStr">
+        <is>
+          <t>Cidade:</t>
+        </is>
+      </c>
+      <c r="E132" t="inlineStr">
+        <is>
+          <t>UF:</t>
+        </is>
+      </c>
+      <c r="F132" t="inlineStr">
+        <is>
+          <t>Empresa:</t>
+        </is>
+      </c>
+      <c r="G132" t="inlineStr">
+        <is>
+          <t>Segmento:</t>
+        </is>
+      </c>
+      <c r="H132" t="inlineStr">
+        <is>
+          <t>CNPJ:</t>
+        </is>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="inlineStr">
+        <is>
+          <t>Nome e Sobrenome:</t>
+        </is>
+      </c>
+      <c r="B133" t="inlineStr">
+        <is>
+          <t>Email:</t>
+        </is>
+      </c>
+      <c r="C133" t="inlineStr">
+        <is>
+          <t>Celular:</t>
+        </is>
+      </c>
+      <c r="D133" t="inlineStr">
+        <is>
+          <t>Cidade:</t>
+        </is>
+      </c>
+      <c r="E133" t="inlineStr">
+        <is>
+          <t>UF:</t>
+        </is>
+      </c>
+      <c r="F133" t="inlineStr">
+        <is>
+          <t>Empresa:</t>
+        </is>
+      </c>
+      <c r="G133" t="inlineStr">
+        <is>
+          <t>Segmento:</t>
+        </is>
+      </c>
+      <c r="H133" t="inlineStr">
+        <is>
+          <t>CNPJ:</t>
+        </is>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" t="inlineStr">
+        <is>
+          <t>Name and Last Name:</t>
+        </is>
+      </c>
+      <c r="B134" t="inlineStr">
+        <is>
+          <t>Email:</t>
+        </is>
+      </c>
+      <c r="C134" t="inlineStr">
+        <is>
+          <t>Phone:</t>
+        </is>
+      </c>
+      <c r="D134" t="inlineStr">
+        <is>
+          <t>City:</t>
+        </is>
+      </c>
+      <c r="E134" t="inlineStr">
+        <is>
+          <t>State:</t>
+        </is>
+      </c>
+      <c r="F134" t="inlineStr">
+        <is>
+          <t>Company:</t>
+        </is>
+      </c>
+      <c r="G134" t="inlineStr">
+        <is>
+          <t>Segment:</t>
+        </is>
+      </c>
+      <c r="H134" t="inlineStr">
+        <is>
+          <t>CNPJ:</t>
+        </is>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="inlineStr">
+        <is>
+          <t>Nome e Sobrenome:</t>
+        </is>
+      </c>
+      <c r="B135" t="inlineStr">
+        <is>
+          <t>Email:</t>
+        </is>
+      </c>
+      <c r="C135" t="inlineStr">
+        <is>
+          <t>Celular:</t>
+        </is>
+      </c>
+      <c r="D135" t="inlineStr">
+        <is>
+          <t>Cidade:</t>
+        </is>
+      </c>
+      <c r="E135" t="inlineStr">
+        <is>
+          <t>UF:</t>
+        </is>
+      </c>
+      <c r="F135" t="inlineStr">
+        <is>
+          <t>Empresa:</t>
+        </is>
+      </c>
+      <c r="G135" t="inlineStr">
+        <is>
+          <t>Segmento:</t>
+        </is>
+      </c>
+      <c r="H135" t="inlineStr">
+        <is>
+          <t>CNPJ:</t>
+        </is>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" t="inlineStr">
+        <is>
+          <t>Nome e Sobrenome:</t>
+        </is>
+      </c>
+      <c r="B136" t="inlineStr">
+        <is>
+          <t>Email:</t>
+        </is>
+      </c>
+      <c r="C136" t="inlineStr">
+        <is>
+          <t>Celular:</t>
+        </is>
+      </c>
+      <c r="D136" t="inlineStr">
+        <is>
+          <t>Cidade:</t>
+        </is>
+      </c>
+      <c r="E136" t="inlineStr">
+        <is>
+          <t>UF:</t>
+        </is>
+      </c>
+      <c r="F136" t="inlineStr">
+        <is>
+          <t>Empresa:</t>
+        </is>
+      </c>
+      <c r="G136" t="inlineStr">
+        <is>
+          <t>Segmento:</t>
+        </is>
+      </c>
+      <c r="H136" t="inlineStr">
+        <is>
+          <t>CNPJ:</t>
+        </is>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" t="inlineStr">
+        <is>
+          <t>Name and Last Name:</t>
+        </is>
+      </c>
+      <c r="B137" t="inlineStr">
+        <is>
+          <t>Email:</t>
+        </is>
+      </c>
+      <c r="C137" t="inlineStr">
+        <is>
+          <t>Phone:</t>
+        </is>
+      </c>
+      <c r="D137" t="inlineStr">
+        <is>
+          <t>City:</t>
+        </is>
+      </c>
+      <c r="E137" t="inlineStr">
+        <is>
+          <t>State:</t>
+        </is>
+      </c>
+      <c r="F137" t="inlineStr">
+        <is>
+          <t>Company:</t>
+        </is>
+      </c>
+      <c r="G137" t="inlineStr">
+        <is>
+          <t>Segment:</t>
+        </is>
+      </c>
+      <c r="H137" t="inlineStr">
+        <is>
+          <t>CNPJ:</t>
+        </is>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" t="inlineStr">
+        <is>
+          <t>Name and Last Name:</t>
+        </is>
+      </c>
+      <c r="B138" t="inlineStr">
+        <is>
+          <t>Email:</t>
+        </is>
+      </c>
+      <c r="C138" t="inlineStr">
+        <is>
+          <t>Phone:</t>
+        </is>
+      </c>
+      <c r="D138" t="inlineStr">
+        <is>
+          <t>City:</t>
+        </is>
+      </c>
+      <c r="E138" t="inlineStr">
+        <is>
+          <t>State:</t>
+        </is>
+      </c>
+      <c r="F138" t="inlineStr">
+        <is>
+          <t>Company:</t>
+        </is>
+      </c>
+      <c r="G138" t="inlineStr">
+        <is>
+          <t>Segment:</t>
+        </is>
+      </c>
+      <c r="H138" t="inlineStr">
+        <is>
+          <t>CNPJ:</t>
+        </is>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" t="inlineStr">
+        <is>
+          <t>Nome e Sobrenome:</t>
+        </is>
+      </c>
+      <c r="B139" t="inlineStr">
+        <is>
+          <t>Email:</t>
+        </is>
+      </c>
+      <c r="C139" t="inlineStr">
+        <is>
+          <t>Celular:</t>
+        </is>
+      </c>
+      <c r="D139" t="inlineStr">
+        <is>
+          <t>Cidade:</t>
+        </is>
+      </c>
+      <c r="E139" t="inlineStr">
+        <is>
+          <t>UF:</t>
+        </is>
+      </c>
+      <c r="F139" t="inlineStr">
+        <is>
+          <t>Empresa:</t>
+        </is>
+      </c>
+      <c r="G139" t="inlineStr">
+        <is>
+          <t>Segmento:</t>
+        </is>
+      </c>
+      <c r="H139" t="inlineStr">
+        <is>
+          <t>CNPJ:</t>
+        </is>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" t="inlineStr">
+        <is>
+          <t>Nome e Sobrenome:</t>
+        </is>
+      </c>
+      <c r="B140" t="inlineStr">
+        <is>
+          <t>Email:</t>
+        </is>
+      </c>
+      <c r="C140" t="inlineStr">
+        <is>
+          <t>Celular:</t>
+        </is>
+      </c>
+      <c r="D140" t="inlineStr">
+        <is>
+          <t>Cidade:</t>
+        </is>
+      </c>
+      <c r="E140" t="inlineStr">
+        <is>
+          <t>UF:</t>
+        </is>
+      </c>
+      <c r="F140" t="inlineStr">
+        <is>
+          <t>Empresa:</t>
+        </is>
+      </c>
+      <c r="G140" t="inlineStr">
+        <is>
+          <t>Segmento:</t>
+        </is>
+      </c>
+      <c r="H140" t="inlineStr">
+        <is>
+          <t>CNPJ:</t>
+        </is>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" t="inlineStr">
+        <is>
+          <t>Nome e Sobrenome:</t>
+        </is>
+      </c>
+      <c r="B141" t="inlineStr">
+        <is>
+          <t>Email:</t>
+        </is>
+      </c>
+      <c r="C141" t="inlineStr">
+        <is>
+          <t>Celular:</t>
+        </is>
+      </c>
+      <c r="D141" t="inlineStr">
+        <is>
+          <t>Cidade:</t>
+        </is>
+      </c>
+      <c r="E141" t="inlineStr">
+        <is>
+          <t>UF:</t>
+        </is>
+      </c>
+      <c r="F141" t="inlineStr">
+        <is>
+          <t>Empresa:</t>
+        </is>
+      </c>
+      <c r="G141" t="inlineStr">
+        <is>
+          <t>Segmento:</t>
+        </is>
+      </c>
+      <c r="H141" t="inlineStr">
+        <is>
+          <t>CNPJ:</t>
+        </is>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" t="inlineStr">
+        <is>
+          <t>Nome e Sobrenome:</t>
+        </is>
+      </c>
+      <c r="B142" t="inlineStr">
+        <is>
+          <t>Email:</t>
+        </is>
+      </c>
+      <c r="C142" t="inlineStr">
+        <is>
+          <t>Celular:</t>
+        </is>
+      </c>
+      <c r="D142" t="inlineStr">
+        <is>
+          <t>Cidade:</t>
+        </is>
+      </c>
+      <c r="E142" t="inlineStr">
+        <is>
+          <t>UF:</t>
+        </is>
+      </c>
+      <c r="F142" t="inlineStr">
+        <is>
+          <t>Empresa:</t>
+        </is>
+      </c>
+      <c r="G142" t="inlineStr">
+        <is>
+          <t>Segmento:</t>
+        </is>
+      </c>
+      <c r="H142" t="inlineStr">
+        <is>
+          <t>CNPJ:</t>
+        </is>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" t="inlineStr">
+        <is>
+          <t>Name and Last Name:</t>
+        </is>
+      </c>
+      <c r="B143" t="inlineStr">
+        <is>
+          <t>Email:</t>
+        </is>
+      </c>
+      <c r="C143" t="inlineStr">
+        <is>
+          <t>Phone:</t>
+        </is>
+      </c>
+      <c r="D143" t="inlineStr">
+        <is>
+          <t>City:</t>
+        </is>
+      </c>
+      <c r="E143" t="inlineStr">
+        <is>
+          <t>State:</t>
+        </is>
+      </c>
+      <c r="F143" t="inlineStr">
+        <is>
+          <t>Company:</t>
+        </is>
+      </c>
+      <c r="G143" t="inlineStr">
+        <is>
+          <t>Segment:</t>
+        </is>
+      </c>
+      <c r="H143" t="inlineStr">
+        <is>
+          <t>CNPJ:</t>
+        </is>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" t="inlineStr">
+        <is>
+          <t>Name and Last Name:</t>
+        </is>
+      </c>
+      <c r="B144" t="inlineStr">
+        <is>
+          <t>Email:</t>
+        </is>
+      </c>
+      <c r="C144" t="inlineStr">
+        <is>
+          <t>Phone:</t>
+        </is>
+      </c>
+      <c r="D144" t="inlineStr">
+        <is>
+          <t>City:</t>
+        </is>
+      </c>
+      <c r="E144" t="inlineStr">
+        <is>
+          <t>State:</t>
+        </is>
+      </c>
+      <c r="F144" t="inlineStr">
+        <is>
+          <t>Company:</t>
+        </is>
+      </c>
+      <c r="G144" t="inlineStr">
+        <is>
+          <t>Segment:</t>
+        </is>
+      </c>
+      <c r="H144" t="inlineStr">
+        <is>
+          <t>CNPJ:</t>
+        </is>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" t="inlineStr">
+        <is>
+          <t>Nome e Sobrenome:</t>
+        </is>
+      </c>
+      <c r="B145" t="inlineStr">
+        <is>
+          <t>Email:</t>
+        </is>
+      </c>
+      <c r="C145" t="inlineStr">
+        <is>
+          <t>Celular:</t>
+        </is>
+      </c>
+      <c r="D145" t="inlineStr">
+        <is>
+          <t>Cidade:</t>
+        </is>
+      </c>
+      <c r="E145" t="inlineStr">
+        <is>
+          <t>UF:</t>
+        </is>
+      </c>
+      <c r="F145" t="inlineStr">
+        <is>
+          <t>Empresa:</t>
+        </is>
+      </c>
+      <c r="G145" t="inlineStr">
+        <is>
+          <t>Segmento:</t>
+        </is>
+      </c>
+      <c r="H145" t="inlineStr">
+        <is>
+          <t>CNPJ:</t>
+        </is>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" t="inlineStr">
+        <is>
+          <t>Name and Last Name:</t>
+        </is>
+      </c>
+      <c r="B146" t="inlineStr">
+        <is>
+          <t>Email:</t>
+        </is>
+      </c>
+      <c r="C146" t="inlineStr">
+        <is>
+          <t>Phone:</t>
+        </is>
+      </c>
+      <c r="D146" t="inlineStr">
+        <is>
+          <t>City:</t>
+        </is>
+      </c>
+      <c r="E146" t="inlineStr">
+        <is>
+          <t>State:</t>
+        </is>
+      </c>
+      <c r="F146" t="inlineStr">
+        <is>
+          <t>Company:</t>
+        </is>
+      </c>
+      <c r="G146" t="inlineStr">
+        <is>
+          <t>Segment:</t>
+        </is>
+      </c>
+      <c r="H146" t="inlineStr">
+        <is>
+          <t>CNPJ:</t>
+        </is>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" t="inlineStr">
+        <is>
+          <t>Name and Last Name:</t>
+        </is>
+      </c>
+      <c r="B147" t="inlineStr">
+        <is>
+          <t>Email:</t>
+        </is>
+      </c>
+      <c r="C147" t="inlineStr">
+        <is>
+          <t>Phone:</t>
+        </is>
+      </c>
+      <c r="D147" t="inlineStr">
+        <is>
+          <t>City:</t>
+        </is>
+      </c>
+      <c r="E147" t="inlineStr">
+        <is>
+          <t>State:</t>
+        </is>
+      </c>
+      <c r="F147" t="inlineStr">
+        <is>
+          <t>Company:</t>
+        </is>
+      </c>
+      <c r="G147" t="inlineStr">
+        <is>
+          <t>Segment:</t>
+        </is>
+      </c>
+      <c r="H147" t="inlineStr">
+        <is>
+          <t>CNPJ:</t>
+        </is>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" t="inlineStr">
+        <is>
+          <t>Name and Last Name:</t>
+        </is>
+      </c>
+      <c r="B148" t="inlineStr">
+        <is>
+          <t>Email:</t>
+        </is>
+      </c>
+      <c r="C148" t="inlineStr">
+        <is>
+          <t>Phone:</t>
+        </is>
+      </c>
+      <c r="D148" t="inlineStr">
+        <is>
+          <t>City:</t>
+        </is>
+      </c>
+      <c r="E148" t="inlineStr">
+        <is>
+          <t>State:</t>
+        </is>
+      </c>
+      <c r="F148" t="inlineStr">
+        <is>
+          <t>Company:</t>
+        </is>
+      </c>
+      <c r="G148" t="inlineStr">
+        <is>
+          <t>Segment:</t>
+        </is>
+      </c>
+      <c r="H148" t="inlineStr">
+        <is>
+          <t>CNPJ:</t>
+        </is>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" t="inlineStr">
+        <is>
+          <t>Name and Last Name:</t>
+        </is>
+      </c>
+      <c r="B149" t="inlineStr">
+        <is>
+          <t>Email:</t>
+        </is>
+      </c>
+      <c r="C149" t="inlineStr">
+        <is>
+          <t>Phone:</t>
+        </is>
+      </c>
+      <c r="D149" t="inlineStr">
+        <is>
+          <t>City:</t>
+        </is>
+      </c>
+      <c r="E149" t="inlineStr">
+        <is>
+          <t>State:</t>
+        </is>
+      </c>
+      <c r="F149" t="inlineStr">
+        <is>
+          <t>Company:</t>
+        </is>
+      </c>
+      <c r="G149" t="inlineStr">
+        <is>
+          <t>Segment:</t>
+        </is>
+      </c>
+      <c r="H149" t="inlineStr">
+        <is>
+          <t>CNPJ:</t>
+        </is>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" t="inlineStr">
+        <is>
+          <t>Nome e Sobrenome:</t>
+        </is>
+      </c>
+      <c r="B150" t="inlineStr">
+        <is>
+          <t>Email:</t>
+        </is>
+      </c>
+      <c r="C150" t="inlineStr">
+        <is>
+          <t>Celular:</t>
+        </is>
+      </c>
+      <c r="D150" t="inlineStr">
+        <is>
+          <t>Cidade:</t>
+        </is>
+      </c>
+      <c r="E150" t="inlineStr">
+        <is>
+          <t>UF:</t>
+        </is>
+      </c>
+      <c r="F150" t="inlineStr">
+        <is>
+          <t>Empresa:</t>
+        </is>
+      </c>
+      <c r="G150" t="inlineStr">
+        <is>
+          <t>Segmento:</t>
+        </is>
+      </c>
+      <c r="H150" t="inlineStr">
+        <is>
+          <t>CNPJ:</t>
+        </is>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" t="inlineStr">
+        <is>
+          <t>Name and Last Name:</t>
+        </is>
+      </c>
+      <c r="B151" t="inlineStr">
+        <is>
+          <t>Email:</t>
+        </is>
+      </c>
+      <c r="C151" t="inlineStr">
+        <is>
+          <t>Phone:</t>
+        </is>
+      </c>
+      <c r="D151" t="inlineStr">
+        <is>
+          <t>City:</t>
+        </is>
+      </c>
+      <c r="E151" t="inlineStr">
+        <is>
+          <t>State:</t>
+        </is>
+      </c>
+      <c r="F151" t="inlineStr">
+        <is>
+          <t>Company:</t>
+        </is>
+      </c>
+      <c r="G151" t="inlineStr">
+        <is>
+          <t>Segment:</t>
+        </is>
+      </c>
+      <c r="H151" t="inlineStr">
+        <is>
+          <t>CNPJ:</t>
+        </is>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" t="inlineStr">
+        <is>
+          <t>Name and Last Name:</t>
+        </is>
+      </c>
+      <c r="B152" t="inlineStr">
+        <is>
+          <t>Email:</t>
+        </is>
+      </c>
+      <c r="C152" t="inlineStr">
+        <is>
+          <t>Phone:</t>
+        </is>
+      </c>
+      <c r="D152" t="inlineStr">
+        <is>
+          <t>City:</t>
+        </is>
+      </c>
+      <c r="E152" t="inlineStr">
+        <is>
+          <t>State:</t>
+        </is>
+      </c>
+      <c r="F152" t="inlineStr">
+        <is>
+          <t>Company:</t>
+        </is>
+      </c>
+      <c r="G152" t="inlineStr">
+        <is>
+          <t>Segment:</t>
+        </is>
+      </c>
+      <c r="H152" t="inlineStr">
+        <is>
+          <t>CNPJ:</t>
+        </is>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" t="inlineStr">
+        <is>
+          <t>Name and Last Name:</t>
+        </is>
+      </c>
+      <c r="B153" t="inlineStr">
+        <is>
+          <t>Email:</t>
+        </is>
+      </c>
+      <c r="C153" t="inlineStr">
+        <is>
+          <t>Phone:</t>
+        </is>
+      </c>
+      <c r="D153" t="inlineStr">
+        <is>
+          <t>City:</t>
+        </is>
+      </c>
+      <c r="E153" t="inlineStr">
+        <is>
+          <t>State:</t>
+        </is>
+      </c>
+      <c r="F153" t="inlineStr">
+        <is>
+          <t>Company:</t>
+        </is>
+      </c>
+      <c r="G153" t="inlineStr">
+        <is>
+          <t>Segment:</t>
+        </is>
+      </c>
+      <c r="H153" t="inlineStr">
+        <is>
+          <t>CNPJ:</t>
+        </is>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" t="inlineStr">
+        <is>
+          <t>Name and Last Name:</t>
+        </is>
+      </c>
+      <c r="B154" t="inlineStr">
+        <is>
+          <t>Email:</t>
+        </is>
+      </c>
+      <c r="C154" t="inlineStr">
+        <is>
+          <t>Phone:</t>
+        </is>
+      </c>
+      <c r="D154" t="inlineStr">
+        <is>
+          <t>City:</t>
+        </is>
+      </c>
+      <c r="E154" t="inlineStr">
+        <is>
+          <t>State:</t>
+        </is>
+      </c>
+      <c r="F154" t="inlineStr">
+        <is>
+          <t>Company:</t>
+        </is>
+      </c>
+      <c r="G154" t="inlineStr">
+        <is>
+          <t>Segment:</t>
+        </is>
+      </c>
+      <c r="H154" t="inlineStr">
+        <is>
+          <t>CNPJ:</t>
+        </is>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" t="inlineStr">
+        <is>
+          <t>Name and Last Name:</t>
+        </is>
+      </c>
+      <c r="B155" t="inlineStr">
+        <is>
+          <t>Email:</t>
+        </is>
+      </c>
+      <c r="C155" t="inlineStr">
+        <is>
+          <t>Phone:</t>
+        </is>
+      </c>
+      <c r="D155" t="inlineStr">
+        <is>
+          <t>City:</t>
+        </is>
+      </c>
+      <c r="E155" t="inlineStr">
+        <is>
+          <t>State:</t>
+        </is>
+      </c>
+      <c r="F155" t="inlineStr">
+        <is>
+          <t>Company:</t>
+        </is>
+      </c>
+      <c r="G155" t="inlineStr">
+        <is>
+          <t>Segment:</t>
+        </is>
+      </c>
+      <c r="H155" t="inlineStr">
+        <is>
+          <t>CNPJ:</t>
+        </is>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" t="inlineStr">
+        <is>
+          <t>Name and Last Name:</t>
+        </is>
+      </c>
+      <c r="B156" t="inlineStr">
+        <is>
+          <t>Email:</t>
+        </is>
+      </c>
+      <c r="C156" t="inlineStr">
+        <is>
+          <t>Phone:</t>
+        </is>
+      </c>
+      <c r="D156" t="inlineStr">
+        <is>
+          <t>City:</t>
+        </is>
+      </c>
+      <c r="E156" t="inlineStr">
+        <is>
+          <t>State:</t>
+        </is>
+      </c>
+      <c r="F156" t="inlineStr">
+        <is>
+          <t>Company:</t>
+        </is>
+      </c>
+      <c r="G156" t="inlineStr">
+        <is>
+          <t>Segment:</t>
+        </is>
+      </c>
+      <c r="H156" t="inlineStr">
+        <is>
+          <t>CNPJ:</t>
+        </is>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" t="inlineStr">
+        <is>
+          <t>Nome e Sobrenome:</t>
+        </is>
+      </c>
+      <c r="B157" t="inlineStr">
+        <is>
+          <t>Email:</t>
+        </is>
+      </c>
+      <c r="C157" t="inlineStr">
+        <is>
+          <t>Celular:</t>
+        </is>
+      </c>
+      <c r="D157" t="inlineStr">
+        <is>
+          <t>Cidade:</t>
+        </is>
+      </c>
+      <c r="E157" t="inlineStr">
+        <is>
+          <t>UF:</t>
+        </is>
+      </c>
+      <c r="F157" t="inlineStr">
+        <is>
+          <t>Empresa:</t>
+        </is>
+      </c>
+      <c r="G157" t="inlineStr">
+        <is>
+          <t>Segmento:</t>
+        </is>
+      </c>
+      <c r="H157" t="inlineStr">
+        <is>
+          <t>CNPJ:</t>
+        </is>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" t="inlineStr">
+        <is>
+          <t>Nome e Sobrenome:</t>
+        </is>
+      </c>
+      <c r="B158" t="inlineStr">
+        <is>
+          <t>Email:</t>
+        </is>
+      </c>
+      <c r="C158" t="inlineStr">
+        <is>
+          <t>Celular:</t>
+        </is>
+      </c>
+      <c r="D158" t="inlineStr">
+        <is>
+          <t>Cidade:</t>
+        </is>
+      </c>
+      <c r="E158" t="inlineStr">
+        <is>
+          <t>UF:</t>
+        </is>
+      </c>
+      <c r="F158" t="inlineStr">
+        <is>
+          <t>Empresa:</t>
+        </is>
+      </c>
+      <c r="G158" t="inlineStr">
+        <is>
+          <t>Segmento:</t>
+        </is>
+      </c>
+      <c r="H158" t="inlineStr">
+        <is>
+          <t>CNPJ:</t>
+        </is>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" t="inlineStr">
+        <is>
+          <t>Name and Last Name:</t>
+        </is>
+      </c>
+      <c r="B159" t="inlineStr">
+        <is>
+          <t>Email:</t>
+        </is>
+      </c>
+      <c r="C159" t="inlineStr">
+        <is>
+          <t>Phone:</t>
+        </is>
+      </c>
+      <c r="D159" t="inlineStr">
+        <is>
+          <t>City:</t>
+        </is>
+      </c>
+      <c r="E159" t="inlineStr">
+        <is>
+          <t>State:</t>
+        </is>
+      </c>
+      <c r="F159" t="inlineStr">
+        <is>
+          <t>Company:</t>
+        </is>
+      </c>
+      <c r="G159" t="inlineStr">
+        <is>
+          <t>Segment:</t>
+        </is>
+      </c>
+      <c r="H159" t="inlineStr">
+        <is>
+          <t>CNPJ:</t>
+        </is>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" t="inlineStr">
+        <is>
+          <t>Name and Last Name:</t>
+        </is>
+      </c>
+      <c r="B160" t="inlineStr">
+        <is>
+          <t>Email:</t>
+        </is>
+      </c>
+      <c r="C160" t="inlineStr">
+        <is>
+          <t>Phone:</t>
+        </is>
+      </c>
+      <c r="D160" t="inlineStr">
+        <is>
+          <t>City:</t>
+        </is>
+      </c>
+      <c r="E160" t="inlineStr">
+        <is>
+          <t>State:</t>
+        </is>
+      </c>
+      <c r="F160" t="inlineStr">
+        <is>
+          <t>Company:</t>
+        </is>
+      </c>
+      <c r="G160" t="inlineStr">
+        <is>
+          <t>Segment:</t>
+        </is>
+      </c>
+      <c r="H160" t="inlineStr">
+        <is>
+          <t>CNPJ:</t>
+        </is>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" t="inlineStr">
+        <is>
+          <t>Nome e Sobrenome:</t>
+        </is>
+      </c>
+      <c r="B161" t="inlineStr">
+        <is>
+          <t>Email:</t>
+        </is>
+      </c>
+      <c r="C161" t="inlineStr">
+        <is>
+          <t>Celular:</t>
+        </is>
+      </c>
+      <c r="D161" t="inlineStr">
+        <is>
+          <t>Cidade:</t>
+        </is>
+      </c>
+      <c r="E161" t="inlineStr">
+        <is>
+          <t>UF:</t>
+        </is>
+      </c>
+      <c r="F161" t="inlineStr">
+        <is>
+          <t>Empresa:</t>
+        </is>
+      </c>
+      <c r="G161" t="inlineStr">
+        <is>
+          <t>Segmento:</t>
+        </is>
+      </c>
+      <c r="H161" t="inlineStr">
+        <is>
+          <t>CNPJ:</t>
+        </is>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" t="inlineStr">
+        <is>
+          <t>Nome e Sobrenome:</t>
+        </is>
+      </c>
+      <c r="B162" t="inlineStr">
+        <is>
+          <t>Email:</t>
+        </is>
+      </c>
+      <c r="C162" t="inlineStr">
+        <is>
+          <t>Celular:</t>
+        </is>
+      </c>
+      <c r="D162" t="inlineStr">
+        <is>
+          <t>Cidade:</t>
+        </is>
+      </c>
+      <c r="E162" t="inlineStr">
+        <is>
+          <t>UF:</t>
+        </is>
+      </c>
+      <c r="F162" t="inlineStr">
+        <is>
+          <t>Empresa:</t>
+        </is>
+      </c>
+      <c r="G162" t="inlineStr">
+        <is>
+          <t>Segmento:</t>
+        </is>
+      </c>
+      <c r="H162" t="inlineStr">
+        <is>
+          <t>CNPJ:</t>
+        </is>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" t="inlineStr">
+        <is>
+          <t>Nome e Sobrenome:</t>
+        </is>
+      </c>
+      <c r="B163" t="inlineStr">
+        <is>
+          <t>Email:</t>
+        </is>
+      </c>
+      <c r="C163" t="inlineStr">
+        <is>
+          <t>Celular:</t>
+        </is>
+      </c>
+      <c r="D163" t="inlineStr">
+        <is>
+          <t>Cidade:</t>
+        </is>
+      </c>
+      <c r="E163" t="inlineStr">
+        <is>
+          <t>UF:</t>
+        </is>
+      </c>
+      <c r="F163" t="inlineStr">
+        <is>
+          <t>Empresa:</t>
+        </is>
+      </c>
+      <c r="G163" t="inlineStr">
+        <is>
+          <t>Segmento:</t>
+        </is>
+      </c>
+      <c r="H163" t="inlineStr">
+        <is>
+          <t>CNPJ:</t>
+        </is>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" t="inlineStr">
+        <is>
+          <t>Name and Last Name:</t>
+        </is>
+      </c>
+      <c r="B164" t="inlineStr">
+        <is>
+          <t>Email:</t>
+        </is>
+      </c>
+      <c r="C164" t="inlineStr">
+        <is>
+          <t>Phone:</t>
+        </is>
+      </c>
+      <c r="D164" t="inlineStr">
+        <is>
+          <t>City:</t>
+        </is>
+      </c>
+      <c r="E164" t="inlineStr">
+        <is>
+          <t>State:</t>
+        </is>
+      </c>
+      <c r="F164" t="inlineStr">
+        <is>
+          <t>Company:</t>
+        </is>
+      </c>
+      <c r="G164" t="inlineStr">
+        <is>
+          <t>Segment:</t>
+        </is>
+      </c>
+      <c r="H164" t="inlineStr">
+        <is>
+          <t>CNPJ:</t>
+        </is>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" t="inlineStr">
+        <is>
+          <t>Name and Last Name:</t>
+        </is>
+      </c>
+      <c r="B165" t="inlineStr">
+        <is>
+          <t>Email:</t>
+        </is>
+      </c>
+      <c r="C165" t="inlineStr">
+        <is>
+          <t>Phone:</t>
+        </is>
+      </c>
+      <c r="D165" t="inlineStr">
+        <is>
+          <t>City:</t>
+        </is>
+      </c>
+      <c r="E165" t="inlineStr">
+        <is>
+          <t>State:</t>
+        </is>
+      </c>
+      <c r="F165" t="inlineStr">
+        <is>
+          <t>Company:</t>
+        </is>
+      </c>
+      <c r="G165" t="inlineStr">
+        <is>
+          <t>Segment:</t>
+        </is>
+      </c>
+      <c r="H165" t="inlineStr">
+        <is>
+          <t>CNPJ:</t>
+        </is>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" t="inlineStr">
+        <is>
+          <t>Name and Last Name:</t>
+        </is>
+      </c>
+      <c r="B166" t="inlineStr">
+        <is>
+          <t>Email:</t>
+        </is>
+      </c>
+      <c r="C166" t="inlineStr">
+        <is>
+          <t>Phone:</t>
+        </is>
+      </c>
+      <c r="D166" t="inlineStr">
+        <is>
+          <t>City:</t>
+        </is>
+      </c>
+      <c r="E166" t="inlineStr">
+        <is>
+          <t>State:</t>
+        </is>
+      </c>
+      <c r="F166" t="inlineStr">
+        <is>
+          <t>Company:</t>
+        </is>
+      </c>
+      <c r="G166" t="inlineStr">
+        <is>
+          <t>Segment:</t>
+        </is>
+      </c>
+      <c r="H166" t="inlineStr">
+        <is>
+          <t>CNPJ:</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
overlay corrigido, tempo mostre resposta correta
</commit_message>
<xml_diff>
--- a/registration_data.xlsx
+++ b/registration_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -559,6 +559,888 @@
         </is>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>h</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>b</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>k</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>l</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>l</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>l</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>k</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>ç</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>+55 (16) 99100-5074</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>CNPJ</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>aa</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>+55 (16) 99100-5074</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>CNPJ</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>b</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>b</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>+55 (16) 99100-5074</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>b</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>b</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>b</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>CNPJ</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>b</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>n</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>n</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>+55 (16) 99100-5074</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>n</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>n</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>n</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>CNPJ</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>n</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>c</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>c</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>+55 (16) 99100-5074</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>c</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>c</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>c</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>CNPJ</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>c</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>d</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>d</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>+55 (16) 99100-5074</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>d</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>d</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>d</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>CNPJ</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>d</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>e</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>e</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>+55 (16) 99100-5074</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>e</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>ee</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>e</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>CNPJ</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>e</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>f</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>f</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>+55 (16) 99100-5074</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>f</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>f</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>f</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>CNPJ</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>f</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>g</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>g</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>16991005074</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>g</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>g</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>g</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>CNPJ</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>g</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>g</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>g</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>+55 (16) 99100-5074</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>g</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>g</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>gg</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>CNPJ</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>g</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>h</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>h</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>16991005074</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>h</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>h</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>h</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>CNPJ</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>h</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>i</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>i</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>16991005074</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>i</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>i</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>i</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>CNPJ</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>i</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>j</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>j</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>+55 (16) 99100-5074</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>j</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>j</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>jj</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>CNPJ</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>j</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>k</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>k</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>16991005074</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>k</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>k</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>kk</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>CNPJ</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>k</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>l</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>ll</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>16991005074</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>l</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>l</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>l</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>CNPJ</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>l</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>m</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>m</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>16991005074</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>m</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>m</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>m</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>CNPJ</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>mm</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>n</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>n</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>16991005074</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>n</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>n</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>n</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>CNPJ</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>n</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>ooo</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>o</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>16991005074</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>o</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>o</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>o</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>CNPJ</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>o</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>p</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>pp</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>16991005074</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>p</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>p</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>p</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>CNPJ</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>p</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>q</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>q</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>+55 (16) 99100-5074</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>q</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>q</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>q</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>CNPJ</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>q</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
part 1 Versão HD
</commit_message>
<xml_diff>
--- a/registration_data.xlsx
+++ b/registration_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H75"/>
+  <dimension ref="A1:H97"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3519,6 +3519,882 @@
         </is>
       </c>
     </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>q</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>q</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>Número inválido</t>
+        </is>
+      </c>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>qq</t>
+        </is>
+      </c>
+      <c r="E76" t="inlineStr">
+        <is>
+          <t>q</t>
+        </is>
+      </c>
+      <c r="F76" t="inlineStr">
+        <is>
+          <t>q</t>
+        </is>
+      </c>
+      <c r="G76" t="inlineStr"/>
+      <c r="H76" t="inlineStr">
+        <is>
+          <t>q</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>q</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>q</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>Número inválido</t>
+        </is>
+      </c>
+      <c r="D77" t="inlineStr">
+        <is>
+          <t>q</t>
+        </is>
+      </c>
+      <c r="E77" t="inlineStr">
+        <is>
+          <t>q</t>
+        </is>
+      </c>
+      <c r="F77" t="inlineStr">
+        <is>
+          <t>qq</t>
+        </is>
+      </c>
+      <c r="G77" t="inlineStr">
+        <is>
+          <t>TAX ID</t>
+        </is>
+      </c>
+      <c r="H77" t="inlineStr">
+        <is>
+          <t>q</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>q</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>q</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>Número inválido</t>
+        </is>
+      </c>
+      <c r="D78" t="inlineStr">
+        <is>
+          <t>q</t>
+        </is>
+      </c>
+      <c r="E78" t="inlineStr">
+        <is>
+          <t>q</t>
+        </is>
+      </c>
+      <c r="F78" t="inlineStr">
+        <is>
+          <t>q</t>
+        </is>
+      </c>
+      <c r="G78" t="inlineStr"/>
+      <c r="H78" t="inlineStr">
+        <is>
+          <t>q</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>q</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>q</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>Número inválido</t>
+        </is>
+      </c>
+      <c r="D79" t="inlineStr">
+        <is>
+          <t>q</t>
+        </is>
+      </c>
+      <c r="E79" t="inlineStr">
+        <is>
+          <t>q</t>
+        </is>
+      </c>
+      <c r="F79" t="inlineStr">
+        <is>
+          <t>q</t>
+        </is>
+      </c>
+      <c r="G79" t="inlineStr">
+        <is>
+          <t>TAX ID</t>
+        </is>
+      </c>
+      <c r="H79" t="inlineStr">
+        <is>
+          <t>q</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>q</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>q</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>Número inválido</t>
+        </is>
+      </c>
+      <c r="D80" t="inlineStr">
+        <is>
+          <t>q</t>
+        </is>
+      </c>
+      <c r="E80" t="inlineStr">
+        <is>
+          <t>q</t>
+        </is>
+      </c>
+      <c r="F80" t="inlineStr">
+        <is>
+          <t>q</t>
+        </is>
+      </c>
+      <c r="G80" t="inlineStr"/>
+      <c r="H80" t="inlineStr">
+        <is>
+          <t>q</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>q</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>q</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>Número inválido</t>
+        </is>
+      </c>
+      <c r="D81" t="inlineStr">
+        <is>
+          <t>q</t>
+        </is>
+      </c>
+      <c r="E81" t="inlineStr">
+        <is>
+          <t>q</t>
+        </is>
+      </c>
+      <c r="F81" t="inlineStr">
+        <is>
+          <t>q</t>
+        </is>
+      </c>
+      <c r="G81" t="inlineStr">
+        <is>
+          <t>TAX ID</t>
+        </is>
+      </c>
+      <c r="H81" t="inlineStr">
+        <is>
+          <t>q</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>q</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>q</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>Número inválido</t>
+        </is>
+      </c>
+      <c r="D82" t="inlineStr">
+        <is>
+          <t>q</t>
+        </is>
+      </c>
+      <c r="E82" t="inlineStr">
+        <is>
+          <t>q</t>
+        </is>
+      </c>
+      <c r="F82" t="inlineStr">
+        <is>
+          <t>q</t>
+        </is>
+      </c>
+      <c r="G82" t="inlineStr"/>
+      <c r="H82" t="inlineStr">
+        <is>
+          <t>q</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>q</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>q</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>Número inválido</t>
+        </is>
+      </c>
+      <c r="D83" t="inlineStr">
+        <is>
+          <t>q</t>
+        </is>
+      </c>
+      <c r="E83" t="inlineStr">
+        <is>
+          <t>q</t>
+        </is>
+      </c>
+      <c r="F83" t="inlineStr">
+        <is>
+          <t>q</t>
+        </is>
+      </c>
+      <c r="G83" t="inlineStr">
+        <is>
+          <t>q</t>
+        </is>
+      </c>
+      <c r="H83" t="inlineStr">
+        <is>
+          <t>q</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>q</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>q</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>Número inválido</t>
+        </is>
+      </c>
+      <c r="D84" t="inlineStr">
+        <is>
+          <t>q</t>
+        </is>
+      </c>
+      <c r="E84" t="inlineStr">
+        <is>
+          <t>q</t>
+        </is>
+      </c>
+      <c r="F84" t="inlineStr">
+        <is>
+          <t>q</t>
+        </is>
+      </c>
+      <c r="G84" t="inlineStr"/>
+      <c r="H84" t="inlineStr">
+        <is>
+          <t>q</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>q</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>q</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>Número inválido</t>
+        </is>
+      </c>
+      <c r="D85" t="inlineStr">
+        <is>
+          <t>q</t>
+        </is>
+      </c>
+      <c r="E85" t="inlineStr">
+        <is>
+          <t>q</t>
+        </is>
+      </c>
+      <c r="F85" t="inlineStr">
+        <is>
+          <t>q</t>
+        </is>
+      </c>
+      <c r="G85" t="inlineStr"/>
+      <c r="H85" t="inlineStr">
+        <is>
+          <t>q</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>q</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>q</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>Número inválido</t>
+        </is>
+      </c>
+      <c r="D86" t="inlineStr">
+        <is>
+          <t>q</t>
+        </is>
+      </c>
+      <c r="E86" t="inlineStr">
+        <is>
+          <t>q</t>
+        </is>
+      </c>
+      <c r="F86" t="inlineStr">
+        <is>
+          <t>q</t>
+        </is>
+      </c>
+      <c r="G86" t="inlineStr">
+        <is>
+          <t>qqq</t>
+        </is>
+      </c>
+      <c r="H86" t="inlineStr">
+        <is>
+          <t>q</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>q</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>q</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>Número inválido</t>
+        </is>
+      </c>
+      <c r="D87" t="inlineStr">
+        <is>
+          <t>q</t>
+        </is>
+      </c>
+      <c r="E87" t="inlineStr">
+        <is>
+          <t>q</t>
+        </is>
+      </c>
+      <c r="F87" t="inlineStr">
+        <is>
+          <t>q</t>
+        </is>
+      </c>
+      <c r="G87" t="inlineStr"/>
+      <c r="H87" t="inlineStr">
+        <is>
+          <t>q</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>h</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>h</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>Número inválido</t>
+        </is>
+      </c>
+      <c r="D88" t="inlineStr">
+        <is>
+          <t>h</t>
+        </is>
+      </c>
+      <c r="E88" t="inlineStr">
+        <is>
+          <t>h</t>
+        </is>
+      </c>
+      <c r="F88" t="inlineStr">
+        <is>
+          <t>h</t>
+        </is>
+      </c>
+      <c r="G88" t="inlineStr">
+        <is>
+          <t>h</t>
+        </is>
+      </c>
+      <c r="H88" t="inlineStr">
+        <is>
+          <t>h</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>w</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>w</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>Número inválido</t>
+        </is>
+      </c>
+      <c r="D89" t="inlineStr">
+        <is>
+          <t>w</t>
+        </is>
+      </c>
+      <c r="E89" t="inlineStr">
+        <is>
+          <t>w</t>
+        </is>
+      </c>
+      <c r="F89" t="inlineStr">
+        <is>
+          <t>w</t>
+        </is>
+      </c>
+      <c r="G89" t="inlineStr"/>
+      <c r="H89" t="inlineStr">
+        <is>
+          <t>w</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>q</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>q</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>Número inválido</t>
+        </is>
+      </c>
+      <c r="D90" t="inlineStr">
+        <is>
+          <t>q</t>
+        </is>
+      </c>
+      <c r="E90" t="inlineStr">
+        <is>
+          <t>q</t>
+        </is>
+      </c>
+      <c r="F90" t="inlineStr">
+        <is>
+          <t>q</t>
+        </is>
+      </c>
+      <c r="G90" t="inlineStr"/>
+      <c r="H90" t="inlineStr">
+        <is>
+          <t>q</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>s</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>s</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>Número inválido</t>
+        </is>
+      </c>
+      <c r="D91" t="inlineStr">
+        <is>
+          <t>s</t>
+        </is>
+      </c>
+      <c r="E91" t="inlineStr">
+        <is>
+          <t>s</t>
+        </is>
+      </c>
+      <c r="F91" t="inlineStr">
+        <is>
+          <t>s</t>
+        </is>
+      </c>
+      <c r="G91" t="inlineStr">
+        <is>
+          <t>s</t>
+        </is>
+      </c>
+      <c r="H91" t="inlineStr">
+        <is>
+          <t>s</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>d</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>d</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>Número inválido</t>
+        </is>
+      </c>
+      <c r="D92" t="inlineStr">
+        <is>
+          <t>d</t>
+        </is>
+      </c>
+      <c r="E92" t="inlineStr">
+        <is>
+          <t>d</t>
+        </is>
+      </c>
+      <c r="F92" t="inlineStr">
+        <is>
+          <t>d</t>
+        </is>
+      </c>
+      <c r="G92" t="inlineStr"/>
+      <c r="H92" t="inlineStr">
+        <is>
+          <t>d</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>ss</t>
+        </is>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>s</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>Número inválido</t>
+        </is>
+      </c>
+      <c r="D93" t="inlineStr">
+        <is>
+          <t>s</t>
+        </is>
+      </c>
+      <c r="E93" t="inlineStr">
+        <is>
+          <t>s</t>
+        </is>
+      </c>
+      <c r="F93" t="inlineStr">
+        <is>
+          <t>s</t>
+        </is>
+      </c>
+      <c r="G93" t="inlineStr">
+        <is>
+          <t>s</t>
+        </is>
+      </c>
+      <c r="H93" t="inlineStr">
+        <is>
+          <t>s</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>s</t>
+        </is>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>s</t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>Número inválido</t>
+        </is>
+      </c>
+      <c r="D94" t="inlineStr">
+        <is>
+          <t>s</t>
+        </is>
+      </c>
+      <c r="E94" t="inlineStr">
+        <is>
+          <t>s</t>
+        </is>
+      </c>
+      <c r="F94" t="inlineStr">
+        <is>
+          <t>s</t>
+        </is>
+      </c>
+      <c r="G94" t="inlineStr"/>
+      <c r="H94" t="inlineStr">
+        <is>
+          <t>s</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>w</t>
+        </is>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>w</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>Número inválido</t>
+        </is>
+      </c>
+      <c r="D95" t="inlineStr">
+        <is>
+          <t>w</t>
+        </is>
+      </c>
+      <c r="E95" t="inlineStr">
+        <is>
+          <t>w</t>
+        </is>
+      </c>
+      <c r="F95" t="inlineStr">
+        <is>
+          <t>w</t>
+        </is>
+      </c>
+      <c r="G95" t="inlineStr">
+        <is>
+          <t>w</t>
+        </is>
+      </c>
+      <c r="H95" t="inlineStr">
+        <is>
+          <t>w</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>d</t>
+        </is>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>d</t>
+        </is>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>Número inválido</t>
+        </is>
+      </c>
+      <c r="D96" t="inlineStr">
+        <is>
+          <t>d</t>
+        </is>
+      </c>
+      <c r="E96" t="inlineStr">
+        <is>
+          <t>d</t>
+        </is>
+      </c>
+      <c r="F96" t="inlineStr">
+        <is>
+          <t>d</t>
+        </is>
+      </c>
+      <c r="G96" t="inlineStr"/>
+      <c r="H96" t="inlineStr">
+        <is>
+          <t>d</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>e</t>
+        </is>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>e</t>
+        </is>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>Número inválido</t>
+        </is>
+      </c>
+      <c r="D97" t="inlineStr">
+        <is>
+          <t>e</t>
+        </is>
+      </c>
+      <c r="E97" t="inlineStr">
+        <is>
+          <t>e</t>
+        </is>
+      </c>
+      <c r="F97" t="inlineStr">
+        <is>
+          <t>e</t>
+        </is>
+      </c>
+      <c r="G97" t="inlineStr">
+        <is>
+          <t>e</t>
+        </is>
+      </c>
+      <c r="H97" t="inlineStr">
+        <is>
+          <t>e</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>